<commit_message>
updated the  t test
</commit_message>
<xml_diff>
--- a/src/mahbub/pair_wise_p_values_Ttest/Statistical_test_for_ranked_feature.xlsx
+++ b/src/mahbub/pair_wise_p_values_Ttest/Statistical_test_for_ranked_feature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28306"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Projects\PycharmProjects\PPMI_Research_on_Parkinson's\src\mahbub\pair_wise_p_values_Ttest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D586FA4-EBE9-42C1-BC45-4AD7A0494B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C43D3F-A148-4C35-9E24-33A6A0E7ACDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="0" windowWidth="21600" windowHeight="16200" xr2:uid="{AEF35B4B-26D0-4411-B03D-0CDA8AECF3E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AEF35B4B-26D0-4411-B03D-0CDA8AECF3E2}"/>
   </bookViews>
   <sheets>
     <sheet name="anova_disease_severity" sheetId="1" r:id="rId1"/>
@@ -714,10 +714,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -765,7 +765,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1098,7 +1109,7 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,22 +1126,22 @@
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="5"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -1858,22 +1869,22 @@
       <c r="A27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="5" t="s">
+      <c r="G27" s="5"/>
+      <c r="H27" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I27" s="5"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2749,14 +2760,14 @@
       <c r="A59" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4" t="s">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E59" s="4"/>
+      <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
@@ -3284,17 +3295,22 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:C26 E3:E26 G3:G26 I3:I26 C28:C57 E28:E57 G28:G57 I28:I57 C61:C90 E61:E90">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>